<commit_message>
updated a mistype of chain-ID in A3
</commit_message>
<xml_diff>
--- a/oldcatv/evidence.xlsx
+++ b/oldcatv/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Documents/Oldcat - validator/Game Of NFT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB156AF-14C6-C84C-A137-4D7292851DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AF9296-4715-674C-B783-656E3A20C770}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="4920" windowWidth="22500" windowHeight="11320" tabRatio="500" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="4920" windowWidth="22500" windowHeight="11320" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -981,7 +981,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1098,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1740,7 +1740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1777,7 +1777,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>